<commit_message>
Remove 2 books from Donated
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="270">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -148,21 +148,6 @@
     <t xml:space="preserve">Numerical analysis; Data processing; Science; Data processing</t>
   </si>
   <si>
-    <t xml:space="preserve">The development of the foundations of mathematical analysis from Euler to Riemann</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grattan-Guinness, I.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-262-07034-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">517/.09/033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematical analysis; History</t>
-  </si>
-  <si>
     <t xml:space="preserve">Differential-difference equations</t>
   </si>
   <si>
@@ -353,18 +338,6 @@
   </si>
   <si>
     <t xml:space="preserve">Computer programming; C (Computer program language)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to symbolic logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pollock, John L.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-03-072765-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logic, Symbolic and mathematical</t>
   </si>
   <si>
     <t xml:space="preserve">Introduction to the constructive theory of functions</t>
@@ -1063,10 +1036,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1350,49 +1323,49 @@
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
+      <c r="C10" s="1" t="n">
+        <v>1963</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>1970</v>
+        <v>1963</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>75110228</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>61018904</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>517.38</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1963</v>
+        <v>1980</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>1963</v>
+        <v>1980</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>61018904</v>
+        <v>79019975</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>517.38</v>
+        <v>574.5</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>28</v>
@@ -1403,57 +1376,57 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="n">
+        <v>1946</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>1980</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>1980</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>79019975</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>574.5</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1968</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>1946</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>55</v>
@@ -1467,80 +1440,80 @@
         <v>57</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>2004</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>2004</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>11</v>
+      <c r="F14" s="1" t="n">
+        <v>2003053836</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1957</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>57000627</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>510.4</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>2004</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>2004</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>2003053836</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>519.4</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1976</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="F16" s="1" t="n">
+        <v>75022015</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1957</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>57000627</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>510.4</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>67</v>
@@ -1557,42 +1530,42 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>1976</v>
+        <v>2009</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>75022015</v>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="n">
+        <v>1993</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>2009</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>11</v>
@@ -1611,113 +1584,113 @@
       <c r="B19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>1993</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>2019</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="n">
+        <v>1964</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1964</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>63021550</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>517.382</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>1971</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1971</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="1" t="n">
+        <v>73149142</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>1964</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>1964</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>63021550</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>517.382</v>
-      </c>
       <c r="H21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="n">
+        <v>78027259</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>73149142</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,7 +1710,7 @@
         <v>95</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>78027259</v>
+        <v>78074114</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>96</v>
@@ -1746,36 +1719,36 @@
         <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1995</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>1979</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>1979</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="n">
+        <v>94048290</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>78074114</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,368 +1758,368 @@
       <c r="B25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>1995</v>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>94048290</v>
+        <v>96009378</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>63020576</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>517.5</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>96009378</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>67023153</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>519</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>69012269</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>63020576</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>517.5</v>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="F29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>67023153</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>519</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>1972</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>1963</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>63020639</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>510.8</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>1978</v>
+        <v>1963</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>63020639</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>510.8</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>124</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1963</v>
+        <v>1968</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>63020639</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>510.8</v>
+        <v>69014427</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>1963</v>
+        <v>2010</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>63020639</v>
+        <v>2009936080</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>510.8</v>
+        <v>519.72</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="F34" s="1" t="n">
+        <v>91003387</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>69014427</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="H34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>2010</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="n">
+        <v>2004050925</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>2009936080</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>519.72</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>1991</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>91003387</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1989</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>2005</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="n">
+        <v>88013897</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="F37" s="1" t="n">
-        <v>2004050925</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>28</v>
@@ -2162,26 +2135,26 @@
       <c r="B38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>11</v>
+      <c r="C38" s="1" t="n">
+        <v>1997</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2019</v>
+        <v>1997</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>11</v>
+      <c r="F38" s="1" t="n">
+        <v>97010390</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,17 +2164,17 @@
       <c r="B39" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
+      <c r="C39" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>1989</v>
+        <v>1971</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>153</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>88013897</v>
+        <v>72127059</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>154</v>
@@ -2220,17 +2193,17 @@
       <c r="B40" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C40" s="1" t="n">
-        <v>1997</v>
+      <c r="C40" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1997</v>
+        <v>1960</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>97010390</v>
+        <v>86029028</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>159</v>
@@ -2239,123 +2212,123 @@
         <v>28</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>1971</v>
+        <v>11</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>69012750</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F41" s="1" t="n">
-        <v>72127059</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <v>1960</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F42" s="1" t="n">
-        <v>86029028</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>168</v>
+        <v>78007594</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>510</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>169</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>90033378</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="1" t="n">
-        <v>69012750</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>67013069</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="H44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F44" s="1" t="n">
-        <v>78007594</v>
-      </c>
-      <c r="G44" s="1" t="n">
-        <v>510</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,46 +2338,46 @@
       <c r="B45" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="1" t="n">
-        <v>1990</v>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F45" s="1" t="n">
-        <v>90033378</v>
+      <c r="F45" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F46" s="1" t="n">
-        <v>67013069</v>
+        <v>82019641</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>182</v>
@@ -2423,150 +2396,150 @@
       <c r="B47" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>11</v>
+      <c r="C47" s="1" t="n">
+        <v>1968</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1991</v>
+        <v>1968</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>68018656</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="n">
+        <v>1977</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>1977</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>78103429</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C48" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D48" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="H48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="F48" s="1" t="n">
-        <v>82019641</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="F49" s="1" t="n">
+        <v>82020810</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>519.4</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D49" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="1" t="n">
-        <v>68018656</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C50" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D50" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F50" s="1" t="n">
-        <v>78103429</v>
+        <v>78008304</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>198</v>
+        <v>96</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>199</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>2006</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D51" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="F51" s="1" t="n">
-        <v>82020810</v>
-      </c>
-      <c r="G51" s="1" t="n">
-        <v>519.4</v>
+        <v>2005937072</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>203</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>1978</v>
@@ -2575,77 +2548,77 @@
         <v>1978</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>78008304</v>
+        <v>78010449</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>101</v>
+        <v>204</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>2006</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="F53" s="1" t="n">
-        <v>2005937072</v>
+        <v>69019015</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>1978</v>
+        <v>1953</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1978</v>
+        <v>1953</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>212</v>
+        <v>11</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>78010449</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>213</v>
+        <v>53008988</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>517.38</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,65 +2626,65 @@
         <v>210</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>69019015</v>
+        <v>88037525</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>1953</v>
+        <v>214</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1953</v>
+        <v>1966</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>53008988</v>
-      </c>
-      <c r="G56" s="1" t="n">
-        <v>517.38</v>
+        <v>66011527</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>11</v>
+        <v>215</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>1989</v>
@@ -2720,85 +2693,85 @@
         <v>1989</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>88037525</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>222</v>
+        <v>89011307</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>220</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>11</v>
+        <v>221</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>1966</v>
+        <v>1969</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>66011527</v>
+        <v>68025426</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>224</v>
+        <v>28</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>59</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>52014012</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>1989</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>1989</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F59" s="1" t="n">
-        <v>89011307</v>
-      </c>
-      <c r="G59" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>1969</v>
@@ -2809,220 +2782,220 @@
       <c r="E60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="1" t="n">
-        <v>68025426</v>
+      <c r="F60" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>231</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>1993</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>93078369</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="1" t="n">
-        <v>52014012</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>1969</v>
+        <v>110</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>1969</v>
+        <v>1964</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>11</v>
+      <c r="F62" s="1" t="n">
+        <v>63020951</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>629.8</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>1993</v>
+        <v>235</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>1962</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F63" s="1" t="n">
-        <v>93078369</v>
+        <v>11</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>240</v>
+        <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>241</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
+        <v>238</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>1961</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F64" s="1" t="n">
-        <v>63020951</v>
+        <v>61018296</v>
       </c>
       <c r="G64" s="1" t="n">
-        <v>629.8</v>
+        <v>531.01</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>120</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>244</v>
+        <v>110</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>11</v>
+        <v>1953</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>1953</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>245</v>
+      <c r="F65" s="1" t="n">
+        <v>53006037</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>1961</v>
+        <v>1970</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1961</v>
+        <v>1970</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>11</v>
+        <v>243</v>
       </c>
       <c r="F66" s="1" t="n">
-        <v>61018296</v>
-      </c>
-      <c r="G66" s="1" t="n">
-        <v>531.01</v>
+        <v>71113604</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="D67" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="1" t="n">
-        <v>53006037</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3032,142 +3005,145 @@
       <c r="B68" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C68" s="1" t="n">
-        <v>1970</v>
+      <c r="C68" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>1970</v>
+        <v>2006</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F68" s="1" t="n">
-        <v>71113604</v>
-      </c>
-      <c r="G68" s="1" t="s">
+        <v>2006000148</v>
+      </c>
+      <c r="G68" s="1" t="n">
+        <v>572.8</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="1" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="1" t="n">
+        <v>62011884</v>
+      </c>
+      <c r="G69" s="1" t="n">
+        <v>510.82</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>1977</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>2006</v>
+        <v>1977</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F70" s="1" t="n">
-        <v>2006000148</v>
-      </c>
-      <c r="G70" s="1" t="n">
-        <v>572.8</v>
+        <v>77082829</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>262</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>1962</v>
+        <v>1996</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>11</v>
+        <v>261</v>
       </c>
       <c r="F71" s="1" t="n">
-        <v>62011884</v>
-      </c>
-      <c r="G71" s="1" t="n">
-        <v>510.82</v>
+        <v>96114475</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="G72" s="1" t="n">
+        <v>72117500</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F72" s="1" t="n">
-        <v>77082829</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="I72" s="1" t="s">
-        <v>128</v>
+        <v>28</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,86 +3153,25 @@
       <c r="B73" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" s="1" t="n">
-        <v>1996</v>
+      <c r="C73" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F73" s="1" t="n">
-        <v>96114475</v>
+        <v>11</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D74" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G74" s="1" t="n">
-        <v>72117500</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I75" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 7a5167fcf32b48065bc602216f0f4c87ccd7f503 🚀
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="270">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -148,21 +148,6 @@
     <t xml:space="preserve">Numerical analysis; Data processing; Science; Data processing</t>
   </si>
   <si>
-    <t xml:space="preserve">The development of the foundations of mathematical analysis from Euler to Riemann</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grattan-Guinness, I.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-262-07034-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">517/.09/033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematical analysis; History</t>
-  </si>
-  <si>
     <t xml:space="preserve">Differential-difference equations</t>
   </si>
   <si>
@@ -353,18 +338,6 @@
   </si>
   <si>
     <t xml:space="preserve">Computer programming; C (Computer program language)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to symbolic logic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pollock, John L.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-03-072765-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logic, Symbolic and mathematical</t>
   </si>
   <si>
     <t xml:space="preserve">Introduction to the constructive theory of functions</t>
@@ -1063,10 +1036,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1350,49 +1323,49 @@
       <c r="B10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
+      <c r="C10" s="1" t="n">
+        <v>1963</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>1970</v>
+        <v>1963</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>75110228</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>45</v>
+        <v>61018904</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>517.38</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1963</v>
+        <v>1980</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>1963</v>
+        <v>1980</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>61018904</v>
+        <v>79019975</v>
       </c>
       <c r="G11" s="1" t="n">
-        <v>517.38</v>
+        <v>574.5</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>28</v>
@@ -1403,57 +1376,57 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="n">
+        <v>1946</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>1980</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>1980</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="1" t="n">
-        <v>79019975</v>
-      </c>
-      <c r="G12" s="1" t="n">
-        <v>574.5</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1968</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>1946</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>55</v>
@@ -1467,80 +1440,80 @@
         <v>57</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>2004</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>2004</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>11</v>
+      <c r="F14" s="1" t="n">
+        <v>2003053836</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>1957</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>57000627</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>510.4</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>2004</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>2004</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>2003053836</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>519.4</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>1976</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="F16" s="1" t="n">
+        <v>75022015</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1957</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>57000627</v>
-      </c>
-      <c r="G16" s="1" t="n">
-        <v>510.4</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>67</v>
@@ -1557,42 +1530,42 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>1976</v>
+        <v>2009</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="1" t="n">
-        <v>75022015</v>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="n">
+        <v>1993</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>2009</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>11</v>
@@ -1611,113 +1584,113 @@
       <c r="B19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="n">
-        <v>1993</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>11</v>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>2019</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="n">
+        <v>1964</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1964</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>63021550</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>517.382</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>1971</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>1971</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="F21" s="1" t="n">
+        <v>73149142</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="1" t="n">
-        <v>1964</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>1964</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F21" s="1" t="n">
-        <v>63021550</v>
-      </c>
-      <c r="G21" s="1" t="n">
-        <v>517.382</v>
-      </c>
       <c r="H21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C22" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="n">
+        <v>78027259</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="1" t="n">
-        <v>73149142</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1737,7 +1710,7 @@
         <v>95</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>78027259</v>
+        <v>78074114</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>96</v>
@@ -1746,36 +1719,36 @@
         <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="n">
+        <v>1995</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>1995</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>1979</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>1979</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="n">
+        <v>94048290</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="1" t="n">
-        <v>78074114</v>
-      </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,368 +1758,368 @@
       <c r="B25" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C25" s="1" t="n">
-        <v>1995</v>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F25" s="1" t="n">
-        <v>94048290</v>
+        <v>96009378</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>63020576</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>517.5</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>96009378</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>67023153</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>519</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>69012269</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>164</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1972</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C28" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F28" s="1" t="n">
-        <v>63020576</v>
-      </c>
-      <c r="G28" s="1" t="n">
-        <v>517.5</v>
+      <c r="G28" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="F29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>67023153</v>
-      </c>
-      <c r="G29" s="1" t="n">
-        <v>519</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C30" s="1" t="n">
-        <v>1972</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>1963</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>63020639</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>510.8</v>
       </c>
       <c r="H30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>1978</v>
+        <v>1963</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>63020639</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>510.8</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>124</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1963</v>
+        <v>1968</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>63020639</v>
-      </c>
-      <c r="G32" s="1" t="n">
-        <v>510.8</v>
+        <v>69014427</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>1963</v>
+        <v>2010</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>11</v>
+        <v>128</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>63020639</v>
+        <v>2009936080</v>
       </c>
       <c r="G33" s="1" t="n">
-        <v>510.8</v>
+        <v>519.72</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>13</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="F34" s="1" t="n">
+        <v>91003387</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>69014427</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="H34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>2010</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="n">
+        <v>2004050925</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F35" s="1" t="n">
-        <v>2009936080</v>
-      </c>
-      <c r="G35" s="1" t="n">
-        <v>519.72</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>1991</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F36" s="1" t="n">
-        <v>91003387</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1989</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>2005</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="n">
+        <v>88013897</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="F37" s="1" t="n">
-        <v>2004050925</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>28</v>
@@ -2162,26 +2135,26 @@
       <c r="B38" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>11</v>
+      <c r="C38" s="1" t="n">
+        <v>1997</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2019</v>
+        <v>1997</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>11</v>
+      <c r="F38" s="1" t="n">
+        <v>97010390</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>11</v>
+        <v>150</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,17 +2164,17 @@
       <c r="B39" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
+      <c r="C39" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>1989</v>
+        <v>1971</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>153</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>88013897</v>
+        <v>72127059</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>154</v>
@@ -2220,17 +2193,17 @@
       <c r="B40" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C40" s="1" t="n">
-        <v>1997</v>
+      <c r="C40" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1997</v>
+        <v>1960</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>158</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>97010390</v>
+        <v>86029028</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>159</v>
@@ -2239,123 +2212,123 @@
         <v>28</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>1971</v>
+        <v>11</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <v>69012750</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="F41" s="1" t="n">
-        <v>72127059</v>
-      </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="1" t="n">
-        <v>1960</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F42" s="1" t="n">
-        <v>86029028</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>168</v>
+        <v>78007594</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>510</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>169</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>90033378</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F43" s="1" t="n">
-        <v>69012750</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>67013069</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="H44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="F44" s="1" t="n">
-        <v>78007594</v>
-      </c>
-      <c r="G44" s="1" t="n">
-        <v>510</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,46 +2338,46 @@
       <c r="B45" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="C45" s="1" t="n">
-        <v>1990</v>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F45" s="1" t="n">
-        <v>90033378</v>
+      <c r="F45" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F46" s="1" t="n">
-        <v>67013069</v>
+        <v>82019641</v>
       </c>
       <c r="G46" s="1" t="s">
         <v>182</v>
@@ -2423,150 +2396,150 @@
       <c r="B47" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>11</v>
+      <c r="C47" s="1" t="n">
+        <v>1968</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1991</v>
+        <v>1968</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>68018656</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="1" t="n">
+        <v>1977</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <v>1977</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>78103429</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C48" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D48" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="H48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="F48" s="1" t="n">
-        <v>82019641</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="F49" s="1" t="n">
+        <v>82020810</v>
+      </c>
+      <c r="G49" s="1" t="n">
+        <v>519.4</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D49" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F49" s="1" t="n">
-        <v>68018656</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C50" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D50" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F50" s="1" t="n">
-        <v>78103429</v>
+        <v>78008304</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>198</v>
+        <v>96</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>199</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <v>2006</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C51" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D51" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>202</v>
-      </c>
       <c r="F51" s="1" t="n">
-        <v>82020810</v>
-      </c>
-      <c r="G51" s="1" t="n">
-        <v>519.4</v>
+        <v>2005937072</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>203</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>1978</v>
@@ -2575,77 +2548,77 @@
         <v>1978</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>78008304</v>
+        <v>78010449</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>101</v>
+        <v>204</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>2006</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="F53" s="1" t="n">
-        <v>2005937072</v>
+        <v>69019015</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>11</v>
+        <v>173</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>128</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>1978</v>
+        <v>1953</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1978</v>
+        <v>1953</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>212</v>
+        <v>11</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>78010449</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>213</v>
+        <v>53008988</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>517.38</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,65 +2626,65 @@
         <v>210</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>69019015</v>
+        <v>88037525</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>182</v>
+        <v>213</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>1953</v>
+        <v>214</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1953</v>
+        <v>1966</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>53008988</v>
-      </c>
-      <c r="G56" s="1" t="n">
-        <v>517.38</v>
+        <v>66011527</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>11</v>
+        <v>215</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>214</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>1989</v>
@@ -2720,85 +2693,85 @@
         <v>1989</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>88037525</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>222</v>
+        <v>89011307</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>59</v>
+        <v>220</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>11</v>
+        <v>221</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>1966</v>
+        <v>1969</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F58" s="1" t="n">
-        <v>66011527</v>
+        <v>68025426</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>224</v>
+        <v>28</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>59</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <v>52014012</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I59" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>1989</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>1989</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="F59" s="1" t="n">
-        <v>89011307</v>
-      </c>
-      <c r="G59" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="H59" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I59" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>1969</v>
@@ -2809,220 +2782,220 @@
       <c r="E60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="1" t="n">
-        <v>68025426</v>
+      <c r="F60" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>231</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>1993</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F61" s="1" t="n">
+        <v>93078369</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="1" t="n">
-        <v>52014012</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>1969</v>
+        <v>110</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>1969</v>
+        <v>1964</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>11</v>
+      <c r="F62" s="1" t="n">
+        <v>63020951</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>629.8</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>1993</v>
+        <v>235</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>1962</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="F63" s="1" t="n">
-        <v>93078369</v>
+        <v>11</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>240</v>
+        <v>13</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>241</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
+        <v>238</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>1961</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F64" s="1" t="n">
-        <v>63020951</v>
+        <v>61018296</v>
       </c>
       <c r="G64" s="1" t="n">
-        <v>629.8</v>
+        <v>531.01</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>120</v>
+        <v>239</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>244</v>
+        <v>110</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>11</v>
+        <v>1953</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <v>1953</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>245</v>
+      <c r="F65" s="1" t="n">
+        <v>53006037</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>1961</v>
+        <v>1970</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1961</v>
+        <v>1970</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>11</v>
+        <v>243</v>
       </c>
       <c r="F66" s="1" t="n">
-        <v>61018296</v>
-      </c>
-      <c r="G66" s="1" t="n">
-        <v>531.01</v>
+        <v>71113604</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>244</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <v>1983</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="D67" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="1" t="n">
-        <v>53006037</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3032,142 +3005,145 @@
       <c r="B68" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C68" s="1" t="n">
-        <v>1970</v>
+      <c r="C68" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>1970</v>
+        <v>2006</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>252</v>
       </c>
       <c r="F68" s="1" t="n">
-        <v>71113604</v>
-      </c>
-      <c r="G68" s="1" t="s">
+        <v>2006000148</v>
+      </c>
+      <c r="G68" s="1" t="n">
+        <v>572.8</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68" s="1" t="s">
         <v>253</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="1" t="n">
+        <v>1962</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="1" t="n">
+        <v>62011884</v>
+      </c>
+      <c r="G69" s="1" t="n">
+        <v>510.82</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D69" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>1977</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>2006</v>
+        <v>1977</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F70" s="1" t="n">
-        <v>2006000148</v>
-      </c>
-      <c r="G70" s="1" t="n">
-        <v>572.8</v>
+        <v>77082829</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>262</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>1962</v>
+        <v>1996</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>11</v>
+        <v>261</v>
       </c>
       <c r="F71" s="1" t="n">
-        <v>62011884</v>
-      </c>
-      <c r="G71" s="1" t="n">
-        <v>510.82</v>
+        <v>96114475</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="E72" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="G72" s="1" t="n">
+        <v>72117500</v>
+      </c>
+      <c r="H72" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="F72" s="1" t="n">
-        <v>77082829</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="I72" s="1" t="s">
-        <v>128</v>
+        <v>28</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3177,86 +3153,25 @@
       <c r="B73" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" s="1" t="n">
-        <v>1996</v>
+      <c r="C73" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F73" s="1" t="n">
-        <v>96114475</v>
+        <v>11</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D74" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G74" s="1" t="n">
-        <v>72117500</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I75" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified book donation pages, Sep 6
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="262">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -382,15 +382,6 @@
     <t xml:space="preserve">Differential equations</t>
   </si>
   <si>
-    <t xml:space="preserve">Lectures on modern mathematics I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saaty, Thomas L.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lectures on modern mathematics II</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lectures on ordinary differential equations</t>
   </si>
   <si>
@@ -704,21 +695,6 @@
   </si>
   <si>
     <t xml:space="preserve">Murray R. Spiegel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The search for E.T. Bell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reid, Constance.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-88385-508-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematicians; Biography; Authors, American; Biography</t>
   </si>
   <si>
     <t xml:space="preserve">Selected papers on mathematical trends in control theory</t>
@@ -1036,10 +1012,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1903,585 +1879,585 @@
       <c r="B30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
+      <c r="C30" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1963</v>
+        <v>1968</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>63020639</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>510.8</v>
+        <v>69014427</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>1963</v>
+        <v>2010</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>63020639</v>
+        <v>2009936080</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>510.8</v>
+        <v>519.72</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>1969</v>
+        <v>128</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1968</v>
+        <v>1991</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>69014427</v>
+        <v>91003387</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>2009936080</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>519.72</v>
+        <v>2004050925</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>91003387</v>
+        <v>137</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>2005</v>
+        <v>1989</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>2004050925</v>
+        <v>88013897</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>1997</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>2019</v>
+        <v>1997</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>11</v>
+        <v>146</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>97010390</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
+        <v>149</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>1989</v>
+        <v>1971</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>88013897</v>
+        <v>72127059</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>1997</v>
+        <v>154</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>1997</v>
+        <v>1960</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>97010390</v>
+        <v>86029028</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>1971</v>
+        <v>11</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>72127059</v>
+        <v>69012750</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1960</v>
+        <v>1978</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>86029028</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>159</v>
+        <v>78007594</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>510</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>11</v>
+        <v>164</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>1990</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>1969</v>
+        <v>1990</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>11</v>
+        <v>165</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>69012750</v>
+        <v>90033378</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1978</v>
+        <v>1967</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>78007594</v>
-      </c>
-      <c r="G42" s="1" t="n">
-        <v>510</v>
+        <v>67013069</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>1990</v>
+        <v>173</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" s="1" t="n">
-        <v>90033378</v>
+        <v>174</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>1983</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>1967</v>
+        <v>1983</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>67013069</v>
+        <v>82019641</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
+        <v>182</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1968</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>1991</v>
+        <v>1968</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>68018656</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>82019641</v>
+        <v>78103429</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>1968</v>
+        <v>1983</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1968</v>
+        <v>1983</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>68018656</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>125</v>
+        <v>82020810</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>78103429</v>
+        <v>78008304</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>1983</v>
+        <v>196</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>1983</v>
+        <v>2006</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>82020810</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <v>519.4</v>
+        <v>2005937072</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>194</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>1978</v>
@@ -2490,19 +2466,19 @@
         <v>1978</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>78008304</v>
+        <v>78010449</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,123 +2486,123 @@
         <v>198</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>11</v>
+        <v>203</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>2006</v>
+        <v>1969</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>2005937072</v>
+        <v>69019015</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>53008988</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>517.38</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F52" s="1" t="n">
-        <v>78010449</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>69019015</v>
+        <v>88037525</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>208</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>1953</v>
+        <v>211</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1953</v>
+        <v>1966</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>53008988</v>
-      </c>
-      <c r="G54" s="1" t="n">
-        <v>517.38</v>
+        <v>66011527</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>205</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>1989</v>
@@ -2635,85 +2611,85 @@
         <v>1989</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>88037525</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>213</v>
+        <v>89011307</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>217</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>11</v>
+        <v>218</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1966</v>
+        <v>1969</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>66011527</v>
+        <v>68025426</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>215</v>
+        <v>28</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>1989</v>
+        <v>221</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>1989</v>
+        <v>1953</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>218</v>
+        <v>11</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>89011307</v>
-      </c>
-      <c r="G57" s="1" t="n">
-        <v>3</v>
+        <v>52014012</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>1969</v>
@@ -2724,46 +2700,46 @@
       <c r="E58" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="1" t="n">
-        <v>68025426</v>
+      <c r="F58" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>222</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>224</v>
+        <v>110</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>1953</v>
+        <v>1964</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F59" s="1" t="n">
-        <v>52014012</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>11</v>
+        <v>63020951</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>629.8</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>225</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,404 +2750,317 @@
         <v>227</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>1969</v>
+        <v>1962</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>11</v>
+        <v>230</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>1961</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>1993</v>
+        <v>1961</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>230</v>
+        <v>11</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>93078369</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
+        <v>61018296</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <v>531.01</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>11</v>
+      <c r="C62" s="1" t="n">
+        <v>1953</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>1964</v>
+        <v>1953</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F62" s="1" t="n">
-        <v>63020951</v>
-      </c>
-      <c r="G62" s="1" t="n">
-        <v>629.8</v>
+        <v>53006037</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="1" t="n">
+        <v>71113604</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H63" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>37</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <v>1961</v>
+        <v>239</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1961</v>
+        <v>1983</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="1" t="n">
-        <v>61018296</v>
-      </c>
-      <c r="G64" s="1" t="n">
-        <v>531.01</v>
+        <v>240</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>1953</v>
+        <v>243</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>1953</v>
+        <v>2006</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>11</v>
+        <v>244</v>
       </c>
       <c r="F65" s="1" t="n">
-        <v>53006037</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>11</v>
+        <v>2006000148</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>572.8</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>119</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>1970</v>
+        <v>247</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1970</v>
+        <v>1962</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>243</v>
+        <v>11</v>
       </c>
       <c r="F66" s="1" t="n">
-        <v>71113604</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>244</v>
+        <v>62011884</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>510.82</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>1977</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>11</v>
+        <v>250</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>77082829</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>249</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>2006</v>
+        <v>1996</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F68" s="1" t="n">
-        <v>2006000148</v>
-      </c>
-      <c r="G68" s="1" t="n">
-        <v>572.8</v>
+        <v>96114475</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>11</v>
+        <v>257</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="1" t="n">
-        <v>62011884</v>
+        <v>1970</v>
+      </c>
+      <c r="E69" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>510.82</v>
+        <v>72117500</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>256</v>
+        <v>28</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>11</v>
+        <v>261</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D70" s="1" t="n">
-        <v>1977</v>
+        <v>1967</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F70" s="1" t="n">
-        <v>77082829</v>
+        <v>11</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F71" s="1" t="n">
-        <v>96114475</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G72" s="1" t="n">
-        <v>72117500</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J72" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 5689f4710b074f1df76397d66052aeed4da66bbc 🚀
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="262">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -382,15 +382,6 @@
     <t xml:space="preserve">Differential equations</t>
   </si>
   <si>
-    <t xml:space="preserve">Lectures on modern mathematics I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saaty, Thomas L.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lectures on modern mathematics II</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lectures on ordinary differential equations</t>
   </si>
   <si>
@@ -704,21 +695,6 @@
   </si>
   <si>
     <t xml:space="preserve">Murray R. Spiegel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The search for E.T. Bell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reid, Constance.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-88385-508-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematicians; Biography; Authors, American; Biography</t>
   </si>
   <si>
     <t xml:space="preserve">Selected papers on mathematical trends in control theory</t>
@@ -1036,10 +1012,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1903,585 +1879,585 @@
       <c r="B30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
+      <c r="C30" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>1963</v>
+        <v>1968</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="1" t="n">
-        <v>63020639</v>
-      </c>
-      <c r="G30" s="1" t="n">
-        <v>510.8</v>
+        <v>69014427</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>13</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>1963</v>
+        <v>2010</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>63020639</v>
+        <v>2009936080</v>
       </c>
       <c r="G31" s="1" t="n">
-        <v>510.8</v>
+        <v>519.72</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>1969</v>
+        <v>128</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1968</v>
+        <v>1991</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>129</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>69014427</v>
+        <v>91003387</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>2009936080</v>
-      </c>
-      <c r="G33" s="1" t="n">
-        <v>519.72</v>
+        <v>2004050925</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>1991</v>
+        <v>2019</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>91003387</v>
+        <v>137</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>2005</v>
+        <v>1989</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>2004050925</v>
+        <v>88013897</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
+        <v>145</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>1997</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>2019</v>
+        <v>1997</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>11</v>
+        <v>146</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <v>97010390</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
+        <v>149</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>1989</v>
+        <v>1971</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>88013897</v>
+        <v>72127059</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>1997</v>
+        <v>154</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>1997</v>
+        <v>1960</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>97010390</v>
+        <v>86029028</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>1971</v>
+        <v>11</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>153</v>
+        <v>11</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>72127059</v>
+        <v>69012750</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1960</v>
+        <v>1978</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>86029028</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>159</v>
+        <v>78007594</v>
+      </c>
+      <c r="G40" s="1" t="n">
+        <v>510</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>160</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>11</v>
+        <v>164</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>1990</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>1969</v>
+        <v>1990</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>11</v>
+        <v>165</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>69012750</v>
+        <v>90033378</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1978</v>
+        <v>1967</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>78007594</v>
-      </c>
-      <c r="G42" s="1" t="n">
-        <v>510</v>
+        <v>67013069</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>13</v>
+        <v>171</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C43" s="1" t="n">
-        <v>1990</v>
+        <v>173</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F43" s="1" t="n">
-        <v>90033378</v>
+        <v>174</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>11</v>
+        <v>177</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>1983</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>1967</v>
+        <v>1983</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>11</v>
+        <v>178</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>67013069</v>
+        <v>82019641</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
+        <v>182</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1968</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>1991</v>
+        <v>1968</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>68018656</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>181</v>
+        <v>11</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>82019641</v>
+        <v>78103429</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>1968</v>
+        <v>1983</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1968</v>
+        <v>1983</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>68018656</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>125</v>
+        <v>82020810</v>
+      </c>
+      <c r="G47" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>78103429</v>
+        <v>78008304</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>189</v>
+        <v>96</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>190</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C49" s="1" t="n">
-        <v>1983</v>
+        <v>196</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>1983</v>
+        <v>2006</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>82020810</v>
-      </c>
-      <c r="G49" s="1" t="n">
-        <v>519.4</v>
+        <v>2005937072</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>194</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="C50" s="1" t="n">
         <v>1978</v>
@@ -2490,19 +2466,19 @@
         <v>1978</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>78008304</v>
+        <v>78010449</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2510,123 +2486,123 @@
         <v>198</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>11</v>
+        <v>203</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>2006</v>
+        <v>1969</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F51" s="1" t="n">
-        <v>2005937072</v>
+        <v>69019015</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>119</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <v>1953</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <v>53008988</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <v>517.38</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F52" s="1" t="n">
-        <v>78010449</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>1969</v>
+        <v>1989</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F53" s="1" t="n">
-        <v>69019015</v>
+        <v>88037525</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>208</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>1953</v>
+        <v>211</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1953</v>
+        <v>1966</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>53008988</v>
-      </c>
-      <c r="G54" s="1" t="n">
-        <v>517.38</v>
+        <v>66011527</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>11</v>
+        <v>212</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>205</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>1989</v>
@@ -2635,85 +2611,85 @@
         <v>1989</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>88037525</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>213</v>
+        <v>89011307</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>54</v>
+        <v>217</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>11</v>
+        <v>218</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1966</v>
+        <v>1969</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>66011527</v>
+        <v>68025426</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>11</v>
+        <v>122</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>215</v>
+        <v>28</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>54</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>1989</v>
+        <v>221</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>1989</v>
+        <v>1953</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>218</v>
+        <v>11</v>
       </c>
       <c r="F57" s="1" t="n">
-        <v>89011307</v>
-      </c>
-      <c r="G57" s="1" t="n">
-        <v>3</v>
+        <v>52014012</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>1969</v>
@@ -2724,46 +2700,46 @@
       <c r="E58" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="1" t="n">
-        <v>68025426</v>
+      <c r="F58" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>222</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>224</v>
+        <v>110</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>1953</v>
+        <v>1964</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F59" s="1" t="n">
-        <v>52014012</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>11</v>
+        <v>63020951</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <v>629.8</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>225</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2774,404 +2750,317 @@
         <v>227</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>1969</v>
+        <v>1962</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>11</v>
+        <v>228</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>11</v>
+        <v>230</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>1961</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>1993</v>
+        <v>1961</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>230</v>
+        <v>11</v>
       </c>
       <c r="F61" s="1" t="n">
-        <v>93078369</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>11</v>
+        <v>61018296</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <v>531.01</v>
       </c>
       <c r="H61" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>11</v>
+      <c r="C62" s="1" t="n">
+        <v>1953</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>1964</v>
+        <v>1953</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F62" s="1" t="n">
-        <v>63020951</v>
-      </c>
-      <c r="G62" s="1" t="n">
-        <v>629.8</v>
+        <v>53006037</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="F63" s="1" t="n">
+        <v>71113604</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H63" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>37</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C64" s="1" t="n">
-        <v>1961</v>
+        <v>239</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>1961</v>
+        <v>1983</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="1" t="n">
-        <v>61018296</v>
-      </c>
-      <c r="G64" s="1" t="n">
-        <v>531.01</v>
+        <v>240</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C65" s="1" t="n">
-        <v>1953</v>
+        <v>243</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>1953</v>
+        <v>2006</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>11</v>
+        <v>244</v>
       </c>
       <c r="F65" s="1" t="n">
-        <v>53006037</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>11</v>
+        <v>2006000148</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>572.8</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>119</v>
+        <v>245</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>1970</v>
+        <v>247</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>1970</v>
+        <v>1962</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>243</v>
+        <v>11</v>
       </c>
       <c r="F66" s="1" t="n">
-        <v>71113604</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>244</v>
+        <v>62011884</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>510.82</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>1977</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>11</v>
+        <v>250</v>
+      </c>
+      <c r="F67" s="1" t="n">
+        <v>77082829</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>249</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>2006</v>
+        <v>1996</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F68" s="1" t="n">
-        <v>2006000148</v>
-      </c>
-      <c r="G68" s="1" t="n">
-        <v>572.8</v>
+        <v>96114475</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>11</v>
+        <v>257</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="1" t="n">
-        <v>62011884</v>
+        <v>1970</v>
+      </c>
+      <c r="E69" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>510.82</v>
+        <v>72117500</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>28</v>
+        <v>259</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>256</v>
+        <v>28</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>11</v>
+        <v>261</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D70" s="1" t="n">
-        <v>1977</v>
+        <v>1967</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F70" s="1" t="n">
-        <v>77082829</v>
+        <v>11</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F71" s="1" t="n">
-        <v>96114475</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="G72" s="1" t="n">
-        <v>72117500</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J72" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed donated books, Sep 11
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="233">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -67,15 +67,6 @@
     <t xml:space="preserve">Real Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">Advanced calculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaplan, Wilfred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Almost Periodic Functions</t>
   </si>
   <si>
@@ -190,18 +181,6 @@
     <t xml:space="preserve">Relativity; Quantum Physics</t>
   </si>
   <si>
-    <t xml:space="preserve">Elementary numerical analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atkinson, Kendall E.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-471-43337-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerical analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve">The enjoyment of mathematics</t>
   </si>
   <si>
@@ -238,21 +217,6 @@
     <t xml:space="preserve">Education; Elementary; Levels; Mathematics; Professional Development; Schools; Subjects; Teaching</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial derivatives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kolb, Robert W.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-13-051559-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93-14127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derivative securities; Financial instruments; Financial futures; Options (Finance); Swaps (Finance); Financial engineering</t>
-  </si>
-  <si>
     <t xml:space="preserve">Financial Mathematics, Derivatives and Structured Products</t>
   </si>
   <si>
@@ -358,18 +322,6 @@
     <t xml:space="preserve">Control theory</t>
   </si>
   <si>
-    <t xml:space="preserve">Introductory Complex Analysis &amp; Applications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William R. Derrick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-12-209950-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70-185029</t>
-  </si>
-  <si>
     <t xml:space="preserve">Isolated invariantsets and the morse index</t>
   </si>
   <si>
@@ -574,18 +526,6 @@
     <t xml:space="preserve">Nonlinear boundary value problems</t>
   </si>
   <si>
-    <t xml:space="preserve">Numerical analysis of spectral methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gottlieb, David; Orszag, Steven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">515.3/5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Differential equations; Numerical solutions; Spectral theory (Mathematics)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Numerical methods, software, and analysis</t>
   </si>
   <si>
@@ -637,24 +577,6 @@
     <t xml:space="preserve">0-03-077455-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Partial differential equations in engineering problems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miller, Kenneth S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partial differential equations of applied mathematics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zauderer, Erich.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-471-61298-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">515.3/53</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resnick, Robert</t>
   </si>
   <si>
@@ -758,15 +680,6 @@
   </si>
   <si>
     <t xml:space="preserve">Biological systems; Mathematical models; Systems biology; Systems Biology; methods; Kinetics; Models, Biological; Models, Statistical; Stochastic Processes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studies in modern analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buck, R. Creighton (Robert Creighton)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematical analysis</t>
   </si>
   <si>
     <t xml:space="preserve">Studies in ordinary differential equations</t>
@@ -1012,10 +925,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1097,36 +1010,36 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1952</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1952</v>
+        <v>1968</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>52007667</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>517</v>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1968</v>
+        <v>1971</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1135,7 +1048,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
@@ -1144,7 +1057,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,72 +1067,72 @@
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1985</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
+      <c r="F5" s="1" t="n">
+        <v>84017860</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>519.2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>1985</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1984</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>84017860</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>519.2</v>
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>1984</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1996</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -1231,120 +1144,120 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>1996</v>
+        <v>1984</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>83021625</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>61018904</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>517.38</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1984</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>83021625</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>519.4</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" s="1" t="n">
-        <v>61018904</v>
+        <v>79019975</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>517.38</v>
+        <v>574.5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1980</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1980</v>
+        <v>1946</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>79019975</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>574.5</v>
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>47</v>
@@ -1358,7 +1271,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1946</v>
+        <v>1968</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -1367,42 +1280,42 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1957</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
+      <c r="F13" s="1" t="n">
+        <v>57000627</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>510.4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>55</v>
@@ -1415,110 +1328,110 @@
       <c r="B14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>2004</v>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>2004</v>
+        <v>1976</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>2003053836</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>519.4</v>
+        <v>75022015</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1957</v>
+        <v>2009</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>57000627</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>510.4</v>
+        <v>63</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1976</v>
+        <v>2019</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>75022015</v>
+        <v>67</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1964</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>2009</v>
+        <v>1964</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>63021550</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>517.382</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>71</v>
@@ -1532,51 +1445,51 @@
         <v>73</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>1993</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>1971</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="1" t="n">
+        <v>73149142</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="n">
+        <v>78027259</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>80</v>
@@ -1590,112 +1503,112 @@
         <v>82</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>1964</v>
+        <v>1979</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>1964</v>
+        <v>1979</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>63021550</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>517.382</v>
+        <v>78074114</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>1971</v>
+        <v>1995</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>1971</v>
+        <v>1995</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>73149142</v>
+        <v>94048290</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>1979</v>
+        <v>91</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>1979</v>
+        <v>1996</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>78027259</v>
+        <v>96009378</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>1979</v>
+        <v>1963</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>1979</v>
+        <v>1963</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>78074114</v>
-      </c>
-      <c r="G23" s="1" t="s">
+        <v>63020576</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>517.5</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,200 +1618,200 @@
       <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>1995</v>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>1995</v>
+        <v>1967</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>67023153</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>519</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <v>94048290</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>96009378</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1968</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>69014427</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>63020576</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>517.5</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="F27" s="1" t="n">
+        <v>2009936080</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>519.72</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>67023153</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>519</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="1" t="n">
-        <v>1972</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="n">
+        <v>91003387</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="n">
+        <v>2004050925</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <v>69014427</v>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,48 +1825,48 @@
         <v>11</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>2010</v>
+        <v>1989</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>2009936080</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>519.72</v>
+        <v>88013897</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>129</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1997</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1991</v>
+        <v>1997</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>91003387</v>
+        <v>97010390</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>127</v>
@@ -1961,260 +1874,260 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>11</v>
+        <v>133</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>2005</v>
+        <v>1971</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>2004050925</v>
+        <v>72127059</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>2019</v>
+        <v>1960</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>86029028</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>1989</v>
+        <v>1969</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>88013897</v>
+        <v>69012750</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>1997</v>
+        <v>11</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>1997</v>
+        <v>1978</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>97010390</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>147</v>
+        <v>78007594</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>510</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>143</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="n">
+        <v>90033378</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F37" s="1" t="n">
-        <v>72127059</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>67013069</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>1960</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F38" s="1" t="n">
-        <v>86029028</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="1" t="n">
-        <v>69012750</v>
+      <c r="F39" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>11</v>
+      <c r="C40" s="1" t="n">
+        <v>1983</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1978</v>
+        <v>1983</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>162</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>78007594</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <v>510</v>
+        <v>82019641</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>1990</v>
+        <v>1968</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>1990</v>
+        <v>1968</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>90033378</v>
+        <v>68018656</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>167</v>
@@ -2227,23 +2140,23 @@
       <c r="B42" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>11</v>
+      <c r="C42" s="1" t="n">
+        <v>1983</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1967</v>
+        <v>1983</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>67013069</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>170</v>
+        <v>82020810</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>171</v>
@@ -2256,237 +2169,237 @@
       <c r="B43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>11</v>
+      <c r="C43" s="1" t="n">
+        <v>1978</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>1991</v>
+        <v>1978</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>11</v>
+      <c r="F43" s="1" t="n">
+        <v>78008304</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>175</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>2006</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="F44" s="1" t="n">
-        <v>82019641</v>
+        <v>2005937072</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>179</v>
+        <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>78010449</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="H45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D45" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="1" t="n">
-        <v>68018656</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F46" s="1" t="n">
-        <v>78103429</v>
+        <v>69019015</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>188</v>
+        <v>51</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>1983</v>
+        <v>185</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1983</v>
+        <v>1966</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>190</v>
+        <v>11</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>82020810</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>519.4</v>
+        <v>66011527</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>11</v>
+        <v>186</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>191</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>1978</v>
+        <v>1989</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>1978</v>
+        <v>1989</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>78008304</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>96</v>
+        <v>89011307</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>11</v>
+        <v>192</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>2006</v>
+        <v>1969</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>197</v>
+        <v>11</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>2005937072</v>
+        <v>68025426</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>1978</v>
+        <v>195</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>1978</v>
+        <v>1953</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>200</v>
+        <v>11</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>78010449</v>
+        <v>52014012</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>1969</v>
@@ -2495,573 +2408,341 @@
         <v>1969</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F51" s="1" t="n">
-        <v>69019015</v>
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>170</v>
+        <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>202</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>1953</v>
+        <v>98</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>1953</v>
+        <v>1964</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>53008988</v>
+        <v>63020951</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>517.38</v>
+        <v>629.8</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>1989</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>1989</v>
+        <v>1962</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F53" s="1" t="n">
-        <v>88037525</v>
+        <v>11</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>210</v>
+        <v>11</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>203</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
+        <v>204</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>1961</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1966</v>
+        <v>1961</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>66011527</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>11</v>
+        <v>61018296</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>531.01</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>212</v>
+        <v>25</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>214</v>
+        <v>98</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>1989</v>
+        <v>1953</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>1989</v>
+        <v>1953</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>215</v>
+        <v>11</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>89011307</v>
-      </c>
-      <c r="G55" s="1" t="n">
-        <v>3</v>
+        <v>53006037</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>216</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>68025426</v>
+        <v>71113604</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>1953</v>
+        <v>1983</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="1" t="n">
-        <v>52014012</v>
+        <v>214</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>1969</v>
+        <v>217</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>1969</v>
+        <v>2006</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>11</v>
+        <v>218</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>2006000148</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <v>572.8</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>11</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>1977</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>1964</v>
+        <v>1977</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="F59" s="1" t="n">
-        <v>63020951</v>
-      </c>
-      <c r="G59" s="1" t="n">
-        <v>629.8</v>
+        <v>77082829</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
+        <v>223</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>1996</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>96114475</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>37</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="G61" s="1" t="n">
+        <v>72117500</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C61" s="1" t="n">
-        <v>1961</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>1961</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="1" t="n">
-        <v>61018296</v>
-      </c>
-      <c r="G61" s="1" t="n">
-        <v>531.01</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="I61" s="1" t="s">
-        <v>231</v>
+        <v>25</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C62" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="D62" s="1" t="n">
-        <v>1953</v>
+        <v>1967</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="1" t="n">
-        <v>53006037</v>
+      <c r="F62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F63" s="1" t="n">
-        <v>71113604</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="1" t="n">
-        <v>2006</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="F65" s="1" t="n">
-        <v>2006000148</v>
-      </c>
-      <c r="G65" s="1" t="n">
-        <v>572.8</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="1" t="n">
-        <v>62011884</v>
-      </c>
-      <c r="G66" s="1" t="n">
-        <v>510.82</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D67" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F67" s="1" t="n">
-        <v>77082829</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F68" s="1" t="n">
-        <v>96114475</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D69" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E69" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G69" s="1" t="n">
-        <v>72117500</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ df1568e3384fc72062b5c1d41d77740d5c400e83 🚀
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="233">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -67,15 +67,6 @@
     <t xml:space="preserve">Real Analysis</t>
   </si>
   <si>
-    <t xml:space="preserve">Advanced calculus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kaplan, Wilfred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calculus</t>
-  </si>
-  <si>
     <t xml:space="preserve">Almost Periodic Functions</t>
   </si>
   <si>
@@ -190,18 +181,6 @@
     <t xml:space="preserve">Relativity; Quantum Physics</t>
   </si>
   <si>
-    <t xml:space="preserve">Elementary numerical analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atkinson, Kendall E.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-471-43337-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerical analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve">The enjoyment of mathematics</t>
   </si>
   <si>
@@ -238,21 +217,6 @@
     <t xml:space="preserve">Education; Elementary; Levels; Mathematics; Professional Development; Schools; Subjects; Teaching</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial derivatives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kolb, Robert W.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-13-051559-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93-14127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derivative securities; Financial instruments; Financial futures; Options (Finance); Swaps (Finance); Financial engineering</t>
-  </si>
-  <si>
     <t xml:space="preserve">Financial Mathematics, Derivatives and Structured Products</t>
   </si>
   <si>
@@ -358,18 +322,6 @@
     <t xml:space="preserve">Control theory</t>
   </si>
   <si>
-    <t xml:space="preserve">Introductory Complex Analysis &amp; Applications</t>
-  </si>
-  <si>
-    <t xml:space="preserve">William R. Derrick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-12-209950-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70-185029</t>
-  </si>
-  <si>
     <t xml:space="preserve">Isolated invariantsets and the morse index</t>
   </si>
   <si>
@@ -574,18 +526,6 @@
     <t xml:space="preserve">Nonlinear boundary value problems</t>
   </si>
   <si>
-    <t xml:space="preserve">Numerical analysis of spectral methods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gottlieb, David; Orszag, Steven</t>
-  </si>
-  <si>
-    <t xml:space="preserve">515.3/5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Differential equations; Numerical solutions; Spectral theory (Mathematics)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Numerical methods, software, and analysis</t>
   </si>
   <si>
@@ -637,24 +577,6 @@
     <t xml:space="preserve">0-03-077455-1</t>
   </si>
   <si>
-    <t xml:space="preserve">Partial differential equations in engineering problems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miller, Kenneth S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partial differential equations of applied mathematics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zauderer, Erich.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-471-61298-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">515.3/53</t>
-  </si>
-  <si>
     <t xml:space="preserve">Resnick, Robert</t>
   </si>
   <si>
@@ -758,15 +680,6 @@
   </si>
   <si>
     <t xml:space="preserve">Biological systems; Mathematical models; Systems biology; Systems Biology; methods; Kinetics; Models, Biological; Models, Statistical; Stochastic Processes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Studies in modern analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buck, R. Creighton (Robert Creighton)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathematical analysis</t>
   </si>
   <si>
     <t xml:space="preserve">Studies in ordinary differential equations</t>
@@ -1012,10 +925,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1097,36 +1010,36 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1952</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1952</v>
+        <v>1968</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>52007667</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>517</v>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1968</v>
+        <v>1971</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>11</v>
@@ -1135,7 +1048,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>11</v>
@@ -1144,7 +1057,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1154,72 +1067,72 @@
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>1985</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
+      <c r="F5" s="1" t="n">
+        <v>84017860</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>519.2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>1985</v>
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1984</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>84017860</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>519.2</v>
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>1984</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1996</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>11</v>
@@ -1231,120 +1144,120 @@
         <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>1996</v>
+        <v>1984</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>83021625</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1963</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>61018904</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>517.38</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>1984</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <v>83021625</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <v>519.4</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1980</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F10" s="1" t="n">
-        <v>61018904</v>
+        <v>79019975</v>
       </c>
       <c r="G10" s="1" t="n">
-        <v>517.38</v>
+        <v>574.5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>1980</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>1980</v>
+        <v>1946</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <v>79019975</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <v>574.5</v>
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>47</v>
@@ -1358,7 +1271,7 @@
         <v>49</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1946</v>
+        <v>1968</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
@@ -1367,42 +1280,42 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1957</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>11</v>
+      <c r="F13" s="1" t="n">
+        <v>57000627</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>510.4</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>54</v>
+        <v>11</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>55</v>
@@ -1415,110 +1328,110 @@
       <c r="B14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="1" t="n">
-        <v>2004</v>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>2004</v>
+        <v>1976</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>2003053836</v>
-      </c>
-      <c r="G14" s="1" t="n">
-        <v>519.4</v>
+        <v>75022015</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>1957</v>
+        <v>2009</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="1" t="n">
-        <v>57000627</v>
-      </c>
-      <c r="G15" s="1" t="n">
-        <v>510.4</v>
+        <v>63</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>1976</v>
+        <v>2019</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="1" t="n">
-        <v>75022015</v>
+        <v>67</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1964</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>2009</v>
+        <v>1964</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>63021550</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>517.382</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>71</v>
@@ -1532,51 +1445,51 @@
         <v>73</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>1993</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>1971</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="1" t="n">
+        <v>73149142</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>1979</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="n">
+        <v>78027259</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>80</v>
@@ -1590,112 +1503,112 @@
         <v>82</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>1964</v>
+        <v>1979</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>1964</v>
+        <v>1979</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>63021550</v>
-      </c>
-      <c r="G20" s="1" t="n">
-        <v>517.382</v>
+        <v>78074114</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>1971</v>
+        <v>1995</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>1971</v>
+        <v>1995</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>73149142</v>
+        <v>94048290</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>1979</v>
+        <v>91</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>1979</v>
+        <v>1996</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F22" s="1" t="n">
-        <v>78027259</v>
+        <v>96009378</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>1979</v>
+        <v>1963</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>1979</v>
+        <v>1963</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="F23" s="1" t="n">
-        <v>78074114</v>
-      </c>
-      <c r="G23" s="1" t="s">
+        <v>63020576</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>517.5</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,200 +1618,200 @@
       <c r="B24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="1" t="n">
-        <v>1995</v>
+      <c r="C24" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>1995</v>
+        <v>1967</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>67023153</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>519</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F24" s="1" t="n">
-        <v>94048290</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>96009378</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>1968</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>69014427</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1963</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F26" s="1" t="n">
-        <v>63020576</v>
-      </c>
-      <c r="G26" s="1" t="n">
-        <v>517.5</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>2010</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="F27" s="1" t="n">
+        <v>2009936080</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>519.72</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F27" s="1" t="n">
-        <v>67023153</v>
-      </c>
-      <c r="G27" s="1" t="n">
-        <v>519</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C28" s="1" t="n">
-        <v>1972</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="n">
+        <v>91003387</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H28" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>2005</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>1978</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="n">
+        <v>2004050925</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>2019</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F30" s="1" t="n">
-        <v>69014427</v>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,48 +1825,48 @@
         <v>11</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>2010</v>
+        <v>1989</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>125</v>
       </c>
       <c r="F31" s="1" t="n">
-        <v>2009936080</v>
-      </c>
-      <c r="G31" s="1" t="n">
-        <v>519.72</v>
+        <v>88013897</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>129</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1997</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>1991</v>
+        <v>1997</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>91003387</v>
+        <v>97010390</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>127</v>
@@ -1961,260 +1874,260 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>11</v>
+        <v>133</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1971</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>2005</v>
+        <v>1971</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F33" s="1" t="n">
-        <v>2004050925</v>
+        <v>72127059</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>2019</v>
+        <v>1960</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>11</v>
+        <v>139</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>86029028</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>11</v>
+        <v>140</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>1989</v>
+        <v>1969</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>88013897</v>
+        <v>69012750</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>1997</v>
+        <v>11</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>1997</v>
+        <v>1978</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>146</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>97010390</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>147</v>
+        <v>78007594</v>
+      </c>
+      <c r="G36" s="1" t="n">
+        <v>510</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>143</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C37" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>1971</v>
-      </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="n">
+        <v>90033378</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F37" s="1" t="n">
-        <v>72127059</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="H37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <v>1967</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <v>67013069</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>1960</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="H38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F38" s="1" t="n">
-        <v>86029028</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="E39" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>1969</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F39" s="1" t="n">
-        <v>69012750</v>
+      <c r="F39" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>11</v>
+      <c r="C40" s="1" t="n">
+        <v>1983</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>1978</v>
+        <v>1983</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>162</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>78007594</v>
-      </c>
-      <c r="G40" s="1" t="n">
-        <v>510</v>
+        <v>82019641</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>1990</v>
+        <v>1968</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>1990</v>
+        <v>1968</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>165</v>
+        <v>11</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>90033378</v>
+        <v>68018656</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>167</v>
@@ -2227,23 +2140,23 @@
       <c r="B42" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>11</v>
+      <c r="C42" s="1" t="n">
+        <v>1983</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>1967</v>
+        <v>1983</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>67013069</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>170</v>
+        <v>82020810</v>
+      </c>
+      <c r="G42" s="1" t="n">
+        <v>519.4</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>171</v>
@@ -2256,237 +2169,237 @@
       <c r="B43" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>11</v>
+      <c r="C43" s="1" t="n">
+        <v>1978</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>1991</v>
+        <v>1978</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>11</v>
+      <c r="F43" s="1" t="n">
+        <v>78008304</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>175</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>2006</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C44" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="D44" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="F44" s="1" t="n">
-        <v>82019641</v>
+        <v>2005937072</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>179</v>
+        <v>11</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>180</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>1978</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>78010449</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="H45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C45" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="D45" s="1" t="n">
-        <v>1968</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F45" s="1" t="n">
-        <v>68018656</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>1969</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C46" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D46" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F46" s="1" t="n">
-        <v>78103429</v>
+        <v>69019015</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>188</v>
+        <v>51</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C47" s="1" t="n">
-        <v>1983</v>
+        <v>185</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>1983</v>
+        <v>1966</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>190</v>
+        <v>11</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>82020810</v>
-      </c>
-      <c r="G47" s="1" t="n">
-        <v>519.4</v>
+        <v>66011527</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>11</v>
+        <v>186</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>191</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>1978</v>
+        <v>1989</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>1978</v>
+        <v>1989</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>78008304</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>96</v>
+        <v>89011307</v>
+      </c>
+      <c r="G48" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>119</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>11</v>
+        <v>192</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1969</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>2006</v>
+        <v>1969</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>197</v>
+        <v>11</v>
       </c>
       <c r="F49" s="1" t="n">
-        <v>2005937072</v>
+        <v>68025426</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C50" s="1" t="n">
-        <v>1978</v>
+        <v>195</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>1978</v>
+        <v>1953</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>200</v>
+        <v>11</v>
       </c>
       <c r="F50" s="1" t="n">
-        <v>78010449</v>
+        <v>52014012</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>201</v>
+        <v>11</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="C51" s="1" t="n">
         <v>1969</v>
@@ -2495,573 +2408,341 @@
         <v>1969</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F51" s="1" t="n">
-        <v>69019015</v>
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>170</v>
+        <v>11</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>202</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>1953</v>
+        <v>98</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>1953</v>
+        <v>1964</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="1" t="n">
-        <v>53008988</v>
+        <v>63020951</v>
       </c>
       <c r="G52" s="1" t="n">
-        <v>517.38</v>
+        <v>629.8</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>1989</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>1989</v>
+        <v>1962</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F53" s="1" t="n">
-        <v>88037525</v>
+        <v>11</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>210</v>
+        <v>11</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>202</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>203</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
+        <v>204</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>1961</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>1966</v>
+        <v>1961</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F54" s="1" t="n">
-        <v>66011527</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>11</v>
+        <v>61018296</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <v>531.01</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>212</v>
+        <v>25</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>214</v>
+        <v>98</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>1989</v>
+        <v>1953</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>1989</v>
+        <v>1953</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>215</v>
+        <v>11</v>
       </c>
       <c r="F55" s="1" t="n">
-        <v>89011307</v>
-      </c>
-      <c r="G55" s="1" t="n">
-        <v>3</v>
+        <v>53006037</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>216</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>11</v>
+        <v>209</v>
       </c>
       <c r="F56" s="1" t="n">
-        <v>68025426</v>
+        <v>71113604</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>122</v>
+        <v>210</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>1953</v>
+        <v>1983</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="1" t="n">
-        <v>52014012</v>
+        <v>214</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>1969</v>
+        <v>217</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>1969</v>
+        <v>2006</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>11</v>
+        <v>218</v>
+      </c>
+      <c r="F58" s="1" t="n">
+        <v>2006000148</v>
+      </c>
+      <c r="G58" s="1" t="n">
+        <v>572.8</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>11</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>11</v>
+        <v>11</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>1977</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>1964</v>
+        <v>1977</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="F59" s="1" t="n">
-        <v>63020951</v>
-      </c>
-      <c r="G59" s="1" t="n">
-        <v>629.8</v>
+        <v>77082829</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
+        <v>223</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <v>1996</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
+      </c>
+      <c r="F60" s="1" t="n">
+        <v>96114475</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>37</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="E61" s="1" t="n">
+        <v>1970</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="G61" s="1" t="n">
+        <v>72117500</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C61" s="1" t="n">
-        <v>1961</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>1961</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F61" s="1" t="n">
-        <v>61018296</v>
-      </c>
-      <c r="G61" s="1" t="n">
-        <v>531.01</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="I61" s="1" t="s">
-        <v>231</v>
+        <v>25</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C62" s="1" t="n">
-        <v>1953</v>
-      </c>
-      <c r="D62" s="1" t="n">
-        <v>1953</v>
+        <v>1967</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="1" t="n">
-        <v>53006037</v>
+      <c r="F62" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="F63" s="1" t="n">
-        <v>71113604</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" s="1" t="n">
-        <v>1983</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="1" t="n">
-        <v>2006</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="F65" s="1" t="n">
-        <v>2006000148</v>
-      </c>
-      <c r="G65" s="1" t="n">
-        <v>572.8</v>
-      </c>
-      <c r="H65" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I65" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="1" t="n">
-        <v>1962</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="1" t="n">
-        <v>62011884</v>
-      </c>
-      <c r="G66" s="1" t="n">
-        <v>510.82</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="D67" s="1" t="n">
-        <v>1977</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="F67" s="1" t="n">
-        <v>77082829</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H67" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="1" t="n">
-        <v>1996</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="F68" s="1" t="n">
-        <v>96114475</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D69" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="E69" s="1" t="n">
-        <v>1970</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="G69" s="1" t="n">
-        <v>72117500</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J69" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>1967</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stochasticdesjulia.pdf, with links
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -927,8 +927,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J52" activeCellId="0" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 408cac1d310c9d096019585bb446f8b611723a90 🚀
</commit_message>
<xml_diff>
--- a/DonatedBooks/donated_books_aug2024.xlsx
+++ b/DonatedBooks/donated_books_aug2024.xlsx
@@ -927,8 +927,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J52" activeCellId="0" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>